<commit_message>
made progress with the zip reader, few bugs
</commit_message>
<xml_diff>
--- a/Version 3.0/extracted_folder/master/COMPUTER_SCIENCE.xlsx
+++ b/Version 3.0/extracted_folder/master/COMPUTER_SCIENCE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Important Files\Final Project\Version 3.0\extracted_folder\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA76FB-0A3D-454D-9954-81B4B54E8C48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B833E87A-7E9B-4627-96F7-CD106BCDC771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="4" xr2:uid="{1EEF0750-3F9E-4F19-8052-8DC30A24F425}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="3" xr2:uid="{1EEF0750-3F9E-4F19-8052-8DC30A24F425}"/>
   </bookViews>
   <sheets>
     <sheet name="100" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>MATH01</t>
   </si>
   <si>
-    <t>CSC01</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>TMC221</t>
   </si>
   <si>
-    <t>MIS01</t>
-  </si>
-  <si>
     <t>SOC01</t>
   </si>
   <si>
@@ -320,6 +314,12 @@
   </si>
   <si>
     <t>DR AKINWUMI SAYO AKINLOYE,DR DUKE ARCHIBONG EYO,DR EJIGA EKO GERALD,DR OBOT NSIKAN IME,DR OJO OLUFEMI FELIX,DR OYEYEMI KEHINDE DAVID,MR ARIJAJE THEOPHILUS EMUOBOR</t>
+  </si>
+  <si>
+    <t>CIS01</t>
+  </si>
+  <si>
+    <t>CMIS01</t>
   </si>
 </sst>
 </file>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FC4050-7AFC-4897-A80A-51F80767416D}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,13 +854,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -877,13 +877,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -897,13 +897,13 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,13 +917,13 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -937,13 +937,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -957,18 +957,18 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -977,18 +977,18 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -997,18 +997,18 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -1017,18 +1017,18 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -1037,18 +1037,18 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1057,18 +1057,18 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -1077,18 +1077,18 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -1097,18 +1097,18 @@
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -1117,13 +1117,13 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F7B39D-A751-4688-92EC-DD4F6F357205}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="B6" zoomScale="59" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.85546875" customWidth="1"/>
+    <col min="4" max="4" width="153.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" customWidth="1"/>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1186,13 +1186,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -1209,18 +1209,18 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1229,18 +1229,18 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -1249,18 +1249,18 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1269,18 +1269,18 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1289,18 +1289,18 @@
         <v>2</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -1309,18 +1309,18 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -1329,18 +1329,18 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>60</v>
@@ -1349,18 +1349,18 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>60</v>
@@ -1369,18 +1369,18 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1389,18 +1389,18 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -1409,18 +1409,18 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -1429,18 +1429,18 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -1449,18 +1449,18 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -1469,18 +1469,18 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -1489,18 +1489,18 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>100</v>
@@ -1509,13 +1509,13 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1575,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EF73E9-BE01-497B-8CBB-DBDD5887B183}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,7 +1584,7 @@
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.85546875" customWidth="1"/>
+    <col min="4" max="4" width="90.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" customWidth="1"/>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1625,13 +1625,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -1648,18 +1648,18 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1668,18 +1668,18 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -1688,18 +1688,18 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1708,18 +1708,18 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1728,18 +1728,18 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -1748,18 +1748,18 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -1768,18 +1768,18 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>40</v>
@@ -1788,18 +1788,18 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1808,18 +1808,18 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1828,18 +1828,18 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -1848,18 +1848,18 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -1868,13 +1868,13 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC11B99F-511C-4906-A3A8-6A298C5747AB}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sorted db creation and population
</commit_message>
<xml_diff>
--- a/Version 3.0/extracted_folder/master/COMPUTER_SCIENCE.xlsx
+++ b/Version 3.0/extracted_folder/master/COMPUTER_SCIENCE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Important Files\Final Project\Version 3.0\extracted_folder\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B833E87A-7E9B-4627-96F7-CD106BCDC771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171FE964-6300-4B79-AE22-E4C51A1F28FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="3" xr2:uid="{1EEF0750-3F9E-4F19-8052-8DC30A24F425}"/>
   </bookViews>
@@ -1576,7 +1576,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>